<commit_message>
Change include QT Design feature
Change include QT Design feature
</commit_message>
<xml_diff>
--- a/contato.xlsx
+++ b/contato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cordon/Drive/Python/gmail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2C1924-6612-D44B-9C13-585A232C0AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB8A2A9-3389-F849-A861-F538B3D5D28A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{536C2E7A-9924-374E-895B-DECBEF862607}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nome</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>Raphael Gmail</t>
-  </si>
-  <si>
-    <t>Denis Nappa</t>
-  </si>
-  <si>
-    <t>denisnappa@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -414,7 +408,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,18 +442,12 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{5F320517-DE37-DA49-AF59-ABA1B5F4156A}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{0BB6B397-3D9D-0B4B-B6CF-697CB6BB13E8}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{B114D5A0-138B-BC41-92F7-54BB2C11E880}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>